<commit_message>
removed valueType categorical from yearly_rep
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_0/1_0_yearly_rep.xlsx
+++ b/dictionaries/urban_ath/1_0/1_0_yearly_rep.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_5E0E3CB4DEABF561B93DB97A10B9B972EF35C7BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAA0C723-EAAE-41FC-BEE4-A79D72148B3D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04352543-4CAE-46AE-9771-8DF7155837CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="311">
   <si>
     <t>name</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>urb_area_id</t>
-  </si>
-  <si>
-    <t>categorical</t>
   </si>
   <si>
     <t>unique identifier for the urban area</t>
@@ -1774,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -1839,1338 +1836,1338 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
         <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>71</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
         <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
         <v>75</v>
       </c>
-      <c r="B33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
         <v>78</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
         <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
         <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>85</v>
-      </c>
-      <c r="D37" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
         <v>87</v>
-      </c>
-      <c r="B38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
         <v>89</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
         <v>91</v>
-      </c>
-      <c r="B40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
         <v>93</v>
-      </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
         <v>95</v>
-      </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
         <v>97</v>
       </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>98</v>
-      </c>
-      <c r="D43" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" t="s">
         <v>100</v>
-      </c>
-      <c r="B44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
         <v>102</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
         <v>104</v>
       </c>
-      <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>105</v>
-      </c>
-      <c r="D46" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
         <v>107</v>
       </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>108</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
         <v>110</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
         <v>112</v>
       </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>113</v>
-      </c>
-      <c r="D49" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s">
         <v>115</v>
-      </c>
-      <c r="B50" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
         <v>117</v>
       </c>
-      <c r="B51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>118</v>
-      </c>
-      <c r="D51" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" t="s">
         <v>120</v>
-      </c>
-      <c r="B52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="s">
         <v>122</v>
-      </c>
-      <c r="B53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
         <v>124</v>
       </c>
-      <c r="B54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>125</v>
-      </c>
-      <c r="D54" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" t="s">
         <v>127</v>
-      </c>
-      <c r="B55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" t="s">
-        <v>125</v>
-      </c>
-      <c r="D55" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" t="s">
         <v>129</v>
-      </c>
-      <c r="B56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" t="s">
         <v>131</v>
-      </c>
-      <c r="B57" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
         <v>133</v>
-      </c>
-      <c r="B58" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
         <v>135</v>
-      </c>
-      <c r="B59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
         <v>137</v>
-      </c>
-      <c r="B60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D60" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D61" t="s">
         <v>139</v>
-      </c>
-      <c r="B61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" t="s">
         <v>141</v>
-      </c>
-      <c r="B62" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" t="s">
         <v>143</v>
-      </c>
-      <c r="B63" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" t="s">
-        <v>98</v>
-      </c>
-      <c r="D63" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64" t="s">
         <v>145</v>
-      </c>
-      <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" t="s">
         <v>147</v>
-      </c>
-      <c r="B65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" t="s">
         <v>149</v>
-      </c>
-      <c r="B66" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
         <v>151</v>
-      </c>
-      <c r="B67" t="s">
-        <v>19</v>
-      </c>
-      <c r="C67" t="s">
-        <v>98</v>
-      </c>
-      <c r="D67" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" t="s">
         <v>153</v>
-      </c>
-      <c r="B68" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" t="s">
-        <v>98</v>
-      </c>
-      <c r="D68" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" t="s">
         <v>155</v>
-      </c>
-      <c r="B69" t="s">
-        <v>19</v>
-      </c>
-      <c r="C69" t="s">
-        <v>98</v>
-      </c>
-      <c r="D69" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>97</v>
+      </c>
+      <c r="D70" t="s">
         <v>157</v>
-      </c>
-      <c r="B70" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" t="s">
-        <v>98</v>
-      </c>
-      <c r="D70" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
+        <v>158</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" t="s">
         <v>159</v>
-      </c>
-      <c r="B71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" t="s">
-        <v>98</v>
-      </c>
-      <c r="D71" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" t="s">
         <v>161</v>
-      </c>
-      <c r="B72" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" t="s">
-        <v>98</v>
-      </c>
-      <c r="D72" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
         <v>163</v>
-      </c>
-      <c r="B73" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
         <v>165</v>
-      </c>
-      <c r="B74" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B75" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" t="s">
         <v>168</v>
-      </c>
-      <c r="D75" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" t="s">
         <v>171</v>
-      </c>
-      <c r="D76" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" t="s">
         <v>173</v>
-      </c>
-      <c r="B77" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D77" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B78" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" t="s">
         <v>176</v>
-      </c>
-      <c r="D78" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
+        <v>177</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B79" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" t="s">
         <v>179</v>
-      </c>
-      <c r="D79" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D80" t="s">
         <v>181</v>
-      </c>
-      <c r="B80" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D80" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" t="s">
         <v>183</v>
-      </c>
-      <c r="B81" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" t="s">
         <v>185</v>
-      </c>
-      <c r="B82" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" t="s">
         <v>187</v>
-      </c>
-      <c r="B83" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" t="s">
-        <v>71</v>
-      </c>
-      <c r="D83" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>117</v>
+      </c>
+      <c r="D84" t="s">
         <v>189</v>
-      </c>
-      <c r="B84" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s">
-        <v>118</v>
-      </c>
-      <c r="D84" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" t="s">
         <v>192</v>
-      </c>
-      <c r="D85" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
+        <v>193</v>
+      </c>
+      <c r="B86" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D86" t="s">
         <v>194</v>
-      </c>
-      <c r="B86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D86" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
+        <v>195</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D87" t="s">
         <v>196</v>
-      </c>
-      <c r="B87" t="s">
-        <v>19</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D87" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
+        <v>97</v>
+      </c>
+      <c r="D88" t="s">
         <v>198</v>
-      </c>
-      <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" t="s">
-        <v>98</v>
-      </c>
-      <c r="D88" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" t="s">
+        <v>97</v>
+      </c>
+      <c r="D89" t="s">
         <v>200</v>
-      </c>
-      <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D89" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
+        <v>201</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D90" t="s">
         <v>202</v>
-      </c>
-      <c r="B90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90" t="s">
-        <v>98</v>
-      </c>
-      <c r="D90" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
+        <v>203</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D91" t="s">
         <v>204</v>
-      </c>
-      <c r="B91" t="s">
-        <v>19</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D91" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D92" t="s">
         <v>206</v>
-      </c>
-      <c r="B92" t="s">
-        <v>19</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D92" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
+        <v>207</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D93" t="s">
         <v>208</v>
-      </c>
-      <c r="B93" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D93" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
+        <v>209</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>97</v>
+      </c>
+      <c r="D94" t="s">
         <v>210</v>
-      </c>
-      <c r="B94" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" t="s">
-        <v>98</v>
-      </c>
-      <c r="D94" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
+        <v>211</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B95" t="s">
-        <v>19</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" t="s">
         <v>213</v>
-      </c>
-      <c r="D95" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
         <v>215</v>
       </c>
-      <c r="B96" t="s">
-        <v>19</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>216</v>
-      </c>
-      <c r="D96" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
+        <v>217</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" t="s">
         <v>218</v>
       </c>
-      <c r="B97" t="s">
-        <v>19</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>219</v>
-      </c>
-      <c r="D97" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
+        <v>220</v>
+      </c>
+      <c r="B98" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B98" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" t="s">
         <v>222</v>
-      </c>
-      <c r="D98" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
+        <v>223</v>
+      </c>
+      <c r="B99" t="s">
+        <v>18</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" t="s">
         <v>224</v>
-      </c>
-      <c r="B99" t="s">
-        <v>19</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D99" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
+        <v>225</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D100" t="s">
         <v>226</v>
-      </c>
-      <c r="B100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D100" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
+        <v>227</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D101" t="s">
         <v>228</v>
-      </c>
-      <c r="B101" t="s">
-        <v>19</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D101" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
+        <v>229</v>
+      </c>
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" t="s">
+        <v>70</v>
+      </c>
+      <c r="D102" t="s">
         <v>230</v>
-      </c>
-      <c r="B102" t="s">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s">
-        <v>71</v>
-      </c>
-      <c r="D102" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -3194,13 +3191,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>232</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>233</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3208,7 +3205,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>30</v>
@@ -3217,12 +3214,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -3231,12 +3228,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>22</v>
@@ -3245,12 +3242,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -3259,12 +3256,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>13</v>
@@ -3273,12 +3270,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3287,12 +3284,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -3301,12 +3298,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -3315,12 +3312,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B10">
         <v>101</v>
@@ -3329,12 +3326,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11">
         <v>102</v>
@@ -3343,12 +3340,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B12">
         <v>103</v>
@@ -3357,12 +3354,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13">
         <v>104</v>
@@ -3371,12 +3368,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B14">
         <v>105</v>
@@ -3385,12 +3382,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15">
         <v>106</v>
@@ -3399,12 +3396,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B16">
         <v>107</v>
@@ -3413,12 +3410,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B17">
         <v>108</v>
@@ -3427,12 +3424,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B18">
         <v>109</v>
@@ -3441,12 +3438,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B19">
         <v>110</v>
@@ -3455,12 +3452,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20">
         <v>111</v>
@@ -3469,12 +3466,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B21">
         <v>112</v>
@@ -3483,12 +3480,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B22">
         <v>113</v>
@@ -3497,12 +3494,12 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B23">
         <v>114</v>
@@ -3511,12 +3508,12 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B24">
         <v>115</v>
@@ -3525,12 +3522,12 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25">
         <v>116</v>
@@ -3539,12 +3536,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B26">
         <v>117</v>
@@ -3553,12 +3550,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B27">
         <v>118</v>
@@ -3567,12 +3564,12 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B28">
         <v>119</v>
@@ -3581,12 +3578,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B29">
         <v>120</v>
@@ -3595,12 +3592,12 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B30">
         <v>121</v>
@@ -3609,12 +3606,12 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B31">
         <v>122</v>
@@ -3623,12 +3620,12 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32">
         <v>123</v>
@@ -3637,12 +3634,12 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B33">
         <v>124</v>
@@ -3651,12 +3648,12 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B34">
         <v>125</v>
@@ -3665,12 +3662,12 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B35">
         <v>126</v>
@@ -3679,12 +3676,12 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B36">
         <v>127</v>
@@ -3693,12 +3690,12 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B37">
         <v>128</v>
@@ -3707,12 +3704,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B38">
         <v>129</v>
@@ -3721,12 +3718,12 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39">
         <v>130</v>
@@ -3735,12 +3732,12 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40">
         <v>131</v>
@@ -3749,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3763,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3777,7 +3774,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3791,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3805,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3819,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3833,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3847,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3861,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3875,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3889,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3903,7 +3900,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3917,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -3931,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3945,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3959,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3973,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3987,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -4001,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -4015,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -4029,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -4043,7 +4040,7 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -4057,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -4071,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -4085,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -4099,12 +4096,12 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4113,12 +4110,12 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -4127,12 +4124,12 @@
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -4141,12 +4138,12 @@
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -4155,12 +4152,12 @@
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -4169,12 +4166,12 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -4183,12 +4180,12 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B72">
         <v>4</v>
@@ -4197,12 +4194,12 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -4211,12 +4208,12 @@
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -4225,12 +4222,12 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -4239,12 +4236,12 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -4253,12 +4250,12 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -4267,12 +4264,12 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B78">
         <v>5</v>
@@ -4281,12 +4278,12 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B79">
         <v>6</v>
@@ -4295,12 +4292,12 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -4309,12 +4306,12 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -4323,12 +4320,12 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -4337,12 +4334,12 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B83">
         <v>4</v>
@@ -4351,12 +4348,12 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B84">
         <v>5</v>
@@ -4365,12 +4362,12 @@
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B85">
         <v>6</v>
@@ -4379,12 +4376,12 @@
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -4393,12 +4390,12 @@
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4407,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>